<commit_message>
Updated Tracking and Backbone Architectures
Tracking works better. There are some problems with user IDs. Implemented Dictionaries instead of np or lists.
</commit_message>
<xml_diff>
--- a/Implementation/ResNet/Scratch/ResNetOnLFWConfigurations.xlsx
+++ b/Implementation/ResNet/Scratch/ResNetOnLFWConfigurations.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e285d3782db16ac6/Desktop/Vicomtech/Repos/TFM_RicardoLuque/Implementation/ResNet/Scratch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="337" documentId="13_ncr:1_{631CBD94-638C-4B98-ADF7-E8C5C3EA406E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{205B9FC4-09C9-42C5-97B9-E3B34C82A1FC}"/>
+  <xr:revisionPtr revIDLastSave="522" documentId="13_ncr:1_{631CBD94-638C-4B98-ADF7-E8C5C3EA406E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{79D4B68B-37C9-475A-9D46-5C8E9AE66CCD}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A1D28061-9B7A-4AF5-B74F-7E502815B0D2}"/>
+    <workbookView xWindow="4800" yWindow="2840" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{A1D28061-9B7A-4AF5-B74F-7E502815B0D2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ResNet50" sheetId="1" r:id="rId1"/>
+    <sheet name="Xception" sheetId="4" r:id="rId2"/>
+    <sheet name="ResNet50V2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="60">
   <si>
     <t>Optimizer</t>
   </si>
@@ -213,12 +216,36 @@
   <si>
     <t>L2</t>
   </si>
+  <si>
+    <t>27 on original size</t>
+  </si>
+  <si>
+    <t>Inout Size</t>
+  </si>
+  <si>
+    <t>71x71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROC AUC </t>
+  </si>
+  <si>
+    <t>ROC AUC/Threshold</t>
+  </si>
+  <si>
+    <t>299x299</t>
+  </si>
+  <si>
+    <t>Not trainable, RAM clashes</t>
+  </si>
+  <si>
+    <t>Size of embeddings</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,6 +271,14 @@
       <color rgb="FF374970"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -314,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -355,13 +390,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -686,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F75E747-9025-4151-9724-B73BBA7EBA5A}">
   <dimension ref="A2:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView topLeftCell="D13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S31" sqref="S31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -711,69 +770,69 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13" t="s">
+      <c r="I2" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13" t="s">
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="13" t="s">
+      <c r="P2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="Q2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="13" t="s">
+      <c r="R2" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="S2" s="13" t="s">
+      <c r="S2" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="T2" s="13" t="s">
+      <c r="T2" s="22" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13" t="s">
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13" t="s">
+      <c r="L3" s="22"/>
+      <c r="M3" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
       <c r="I4" s="1" t="s">
         <v>1</v>
       </c>
@@ -792,12 +851,12 @@
       <c r="N4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
@@ -839,7 +898,7 @@
       <c r="R5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S5" s="13" t="s">
+      <c r="S5" s="22" t="s">
         <v>31</v>
       </c>
       <c r="T5" s="11" t="s">
@@ -883,7 +942,7 @@
       <c r="R6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S6" s="13"/>
+      <c r="S6" s="22"/>
       <c r="T6" s="11" t="s">
         <v>32</v>
       </c>
@@ -925,7 +984,7 @@
       <c r="R7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S7" s="13"/>
+      <c r="S7" s="22"/>
       <c r="T7" s="1" t="s">
         <v>33</v>
       </c>
@@ -973,7 +1032,7 @@
       <c r="R8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S8" s="13"/>
+      <c r="S8" s="22"/>
       <c r="T8" s="1" t="s">
         <v>34</v>
       </c>
@@ -1021,7 +1080,7 @@
       <c r="R9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S9" s="13"/>
+      <c r="S9" s="22"/>
       <c r="T9" s="1" t="s">
         <v>35</v>
       </c>
@@ -1069,7 +1128,7 @@
       <c r="R10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S10" s="13"/>
+      <c r="S10" s="22"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="E11" s="1">
@@ -1114,7 +1173,7 @@
       <c r="R11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S11" s="13"/>
+      <c r="S11" s="22"/>
       <c r="T11" s="1" t="s">
         <v>36</v>
       </c>
@@ -1162,7 +1221,7 @@
       <c r="R12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S12" s="13"/>
+      <c r="S12" s="22"/>
       <c r="T12" s="1" t="s">
         <v>37</v>
       </c>
@@ -1210,7 +1269,7 @@
       <c r="R13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S13" s="13"/>
+      <c r="S13" s="22"/>
       <c r="T13" s="1" t="s">
         <v>38</v>
       </c>
@@ -1258,7 +1317,7 @@
       <c r="R14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S14" s="13"/>
+      <c r="S14" s="22"/>
       <c r="T14" s="1" t="s">
         <v>39</v>
       </c>
@@ -1306,7 +1365,7 @@
       <c r="R15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S15" s="13"/>
+      <c r="S15" s="22"/>
       <c r="T15" s="10" t="s">
         <v>40</v>
       </c>
@@ -1354,7 +1413,7 @@
       <c r="R16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S16" s="13"/>
+      <c r="S16" s="22"/>
     </row>
     <row r="17" spans="5:20" ht="20.5" x14ac:dyDescent="0.35">
       <c r="E17" s="1">
@@ -1399,7 +1458,7 @@
       <c r="R17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="S17" s="13"/>
+      <c r="S17" s="22"/>
       <c r="T17" s="10" t="s">
         <v>41</v>
       </c>
@@ -1447,7 +1506,7 @@
       <c r="R18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="S18" s="13"/>
+      <c r="S18" s="22"/>
       <c r="T18" s="11" t="s">
         <v>42</v>
       </c>
@@ -1495,7 +1554,7 @@
       <c r="R19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="S19" s="13"/>
+      <c r="S19" s="22"/>
     </row>
     <row r="20" spans="5:20" x14ac:dyDescent="0.35">
       <c r="E20" s="1">
@@ -1540,7 +1599,7 @@
       <c r="R20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="S20" s="13"/>
+      <c r="S20" s="22"/>
       <c r="T20" s="1" t="s">
         <v>44</v>
       </c>
@@ -1588,7 +1647,7 @@
       <c r="R21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="S21" s="13"/>
+      <c r="S21" s="22"/>
       <c r="T21" s="1" t="s">
         <v>45</v>
       </c>
@@ -1636,7 +1695,7 @@
       <c r="R22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="S22" s="13"/>
+      <c r="S22" s="22"/>
     </row>
     <row r="23" spans="5:20" x14ac:dyDescent="0.35">
       <c r="E23" s="1">
@@ -1681,7 +1740,7 @@
       <c r="R23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="S23" s="13"/>
+      <c r="S23" s="22"/>
       <c r="T23" s="1" t="s">
         <v>46</v>
       </c>
@@ -1729,7 +1788,7 @@
       <c r="R24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="S24" s="13"/>
+      <c r="S24" s="22"/>
     </row>
     <row r="25" spans="5:20" x14ac:dyDescent="0.35">
       <c r="E25" s="1">
@@ -1750,16 +1809,16 @@
       <c r="J25" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K25" s="16">
+      <c r="K25" s="15">
         <v>0.94021999999999994</v>
       </c>
-      <c r="L25" s="16">
+      <c r="L25" s="15">
         <v>1</v>
       </c>
-      <c r="M25" s="16">
+      <c r="M25" s="15">
         <v>0.48199999999999998</v>
       </c>
-      <c r="N25" s="16">
+      <c r="N25" s="15">
         <v>0.77639999999999998</v>
       </c>
       <c r="O25" s="1" t="s">
@@ -1774,7 +1833,7 @@
       <c r="R25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="S25" s="13"/>
+      <c r="S25" s="22"/>
     </row>
     <row r="26" spans="5:20" x14ac:dyDescent="0.35">
       <c r="E26" s="1">
@@ -1819,7 +1878,7 @@
       <c r="R26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="S26" s="13"/>
+      <c r="S26" s="22"/>
     </row>
     <row r="27" spans="5:20" x14ac:dyDescent="0.35">
       <c r="E27" s="1">
@@ -1831,7 +1890,7 @@
       <c r="G27" s="1">
         <v>100</v>
       </c>
-      <c r="H27" s="14" t="s">
+      <c r="H27" s="23" t="s">
         <v>16</v>
       </c>
       <c r="I27" s="1">
@@ -1864,7 +1923,7 @@
       <c r="R27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="S27" s="13" t="s">
+      <c r="S27" s="22" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1878,7 +1937,7 @@
       <c r="G28" s="8">
         <v>100</v>
       </c>
-      <c r="H28" s="14"/>
+      <c r="H28" s="23"/>
       <c r="I28" s="8">
         <v>1E-3</v>
       </c>
@@ -1909,7 +1968,7 @@
       <c r="R28" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="S28" s="13"/>
+      <c r="S28" s="22"/>
     </row>
     <row r="29" spans="5:20" x14ac:dyDescent="0.35">
       <c r="E29" s="8">
@@ -1921,7 +1980,7 @@
       <c r="G29" s="8">
         <v>100</v>
       </c>
-      <c r="H29" s="14"/>
+      <c r="H29" s="23"/>
       <c r="I29" s="8">
         <v>1E-3</v>
       </c>
@@ -1966,7 +2025,7 @@
       <c r="G30" s="8">
         <v>100</v>
       </c>
-      <c r="H30" s="14"/>
+      <c r="H30" s="23"/>
       <c r="I30" s="8">
         <v>1E-3</v>
       </c>
@@ -2011,39 +2070,39 @@
       <c r="G31" s="12">
         <v>100</v>
       </c>
-      <c r="H31" s="14"/>
-      <c r="I31" s="15">
+      <c r="H31" s="23"/>
+      <c r="I31" s="14">
         <v>1E-3</v>
       </c>
-      <c r="J31" s="15" t="s">
+      <c r="J31" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="K31" s="15">
+      <c r="K31" s="14">
         <v>0.92859999999999998</v>
       </c>
-      <c r="L31" s="15">
+      <c r="L31" s="14">
         <v>1</v>
       </c>
-      <c r="M31" s="15">
+      <c r="M31" s="14">
         <v>0.63139999999999996</v>
       </c>
-      <c r="N31" s="15">
+      <c r="N31" s="14">
         <v>0.84179999999999999</v>
       </c>
-      <c r="O31" s="8" t="s">
+      <c r="O31" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="P31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q31" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="R31" s="8" t="s">
+      <c r="P31" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q31" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="R31" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="S31" s="1" t="s">
-        <v>29</v>
+      <c r="S31" s="21" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="5:20" x14ac:dyDescent="0.35">
@@ -2056,7 +2115,7 @@
       <c r="G32" s="8">
         <v>100</v>
       </c>
-      <c r="H32" s="14"/>
+      <c r="H32" s="23"/>
       <c r="I32" s="1">
         <v>1E-3</v>
       </c>
@@ -2088,7 +2147,7 @@
         <v>23</v>
       </c>
       <c r="S32" s="1" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="5:19" x14ac:dyDescent="0.35">
@@ -2101,7 +2160,7 @@
       <c r="G33" s="8">
         <v>100</v>
       </c>
-      <c r="H33" s="14"/>
+      <c r="H33" s="23"/>
       <c r="I33" s="9">
         <v>1E-4</v>
       </c>
@@ -2146,7 +2205,7 @@
       <c r="G34" s="8">
         <v>100</v>
       </c>
-      <c r="H34" s="14"/>
+      <c r="H34" s="23"/>
       <c r="I34" s="9">
         <v>1E-4</v>
       </c>
@@ -2191,7 +2250,7 @@
       <c r="G35" s="8">
         <v>100</v>
       </c>
-      <c r="H35" s="14"/>
+      <c r="H35" s="23"/>
       <c r="I35" s="9">
         <v>1E-4</v>
       </c>
@@ -2236,7 +2295,7 @@
       <c r="G36" s="8">
         <v>100</v>
       </c>
-      <c r="H36" s="14"/>
+      <c r="H36" s="23"/>
       <c r="I36" s="9">
         <v>1E-4</v>
       </c>
@@ -2273,11 +2332,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="T2:T4"/>
-    <mergeCell ref="S2:S4"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="K2:N2"/>
     <mergeCell ref="S5:S26"/>
     <mergeCell ref="S27:S28"/>
     <mergeCell ref="H27:H36"/>
@@ -2289,9 +2343,771 @@
     <mergeCell ref="I2:J3"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="M3:N3"/>
+    <mergeCell ref="T2:T4"/>
+    <mergeCell ref="S2:S4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="K2:N2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11A6DBAE-626E-4512-B6E6-0825E56A59F1}">
+  <dimension ref="B2:Q9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="8" width="8.7265625" style="16"/>
+    <col min="9" max="9" width="7" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.26953125" style="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.81640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.54296875" style="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.6328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9" style="16" customWidth="1"/>
+    <col min="16" max="16" width="17.7265625" style="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.7265625" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B2" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="P2" s="24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B5" s="17">
+        <v>27</v>
+      </c>
+      <c r="C5" s="17">
+        <v>64</v>
+      </c>
+      <c r="D5" s="17">
+        <v>100</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="17">
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="G5" s="17">
+        <v>1</v>
+      </c>
+      <c r="H5" s="17">
+        <v>0.73680000000000001</v>
+      </c>
+      <c r="I5" s="17">
+        <v>0.876</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="17">
+        <v>1024</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="M5" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="O5" s="16">
+        <v>0.99695699999999998</v>
+      </c>
+      <c r="P5" s="16">
+        <v>0.88203500000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B6" s="17">
+        <v>27</v>
+      </c>
+      <c r="C6" s="17">
+        <v>64</v>
+      </c>
+      <c r="D6" s="17">
+        <v>100</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="17">
+        <v>0.95850000000000002</v>
+      </c>
+      <c r="G6" s="17">
+        <v>1</v>
+      </c>
+      <c r="H6" s="17">
+        <v>0.75370000000000004</v>
+      </c>
+      <c r="I6" s="17">
+        <v>0.89080000000000004</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="17">
+        <v>512</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="M6" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="O6" s="16">
+        <v>0.997587</v>
+      </c>
+      <c r="P6" s="16">
+        <v>0.89490000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B7" s="17">
+        <v>27</v>
+      </c>
+      <c r="C7" s="17">
+        <v>64</v>
+      </c>
+      <c r="D7" s="17">
+        <v>100</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="16">
+        <v>0.96450000000000002</v>
+      </c>
+      <c r="G7" s="16">
+        <v>1</v>
+      </c>
+      <c r="H7" s="16">
+        <v>0.75880000000000003</v>
+      </c>
+      <c r="I7" s="16">
+        <v>0.8992</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="17">
+        <v>256</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="M7" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="O7" s="16">
+        <v>0.99803200000000003</v>
+      </c>
+      <c r="P7" s="16">
+        <v>0.90959500000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="K8" s="16">
+        <v>1024</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q8" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="K9" s="16">
+        <v>512</v>
+      </c>
+      <c r="L9" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="O2:O4"/>
+    <mergeCell ref="P2:P4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="N2:N4"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C523007-AF36-4B4A-8C32-57E4C8F48C0E}">
+  <dimension ref="E2:R14"/>
+  <sheetViews>
+    <sheetView topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:R12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="4" width="8.7265625" style="13"/>
+    <col min="5" max="5" width="15.7265625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.7265625" style="13"/>
+    <col min="8" max="8" width="31.6328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7265625" style="13"/>
+    <col min="10" max="10" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.54296875" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.54296875" style="13" customWidth="1"/>
+    <col min="13" max="13" width="14.453125" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.90625" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.453125" style="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.6328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.26953125" style="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.26953125" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="86.7265625" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.7265625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="5:18" x14ac:dyDescent="0.35">
+      <c r="E2" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2" s="24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="5:18" x14ac:dyDescent="0.35">
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24"/>
+    </row>
+    <row r="4" spans="5:18" x14ac:dyDescent="0.35">
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+    </row>
+    <row r="5" spans="5:18" x14ac:dyDescent="0.35">
+      <c r="E5" s="8">
+        <v>25</v>
+      </c>
+      <c r="F5" s="8">
+        <v>64</v>
+      </c>
+      <c r="G5" s="8">
+        <v>100</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="17">
+        <v>0.86050000000000004</v>
+      </c>
+      <c r="J5" s="17">
+        <v>1</v>
+      </c>
+      <c r="K5" s="17">
+        <v>0.58599999999999997</v>
+      </c>
+      <c r="L5" s="17">
+        <v>0.78259999999999996</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="O5" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q5" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="5:18" x14ac:dyDescent="0.35">
+      <c r="E6" s="8">
+        <v>26</v>
+      </c>
+      <c r="F6" s="8">
+        <v>64</v>
+      </c>
+      <c r="G6" s="8">
+        <v>100</v>
+      </c>
+      <c r="H6" s="23"/>
+      <c r="I6" s="17">
+        <v>0.87239999999999995</v>
+      </c>
+      <c r="J6" s="17">
+        <v>1</v>
+      </c>
+      <c r="K6" s="17">
+        <v>0.59940000000000004</v>
+      </c>
+      <c r="L6" s="17">
+        <v>0.75119999999999998</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="O6" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q6" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="5:18" x14ac:dyDescent="0.35">
+      <c r="E7" s="12">
+        <v>27</v>
+      </c>
+      <c r="F7" s="12">
+        <v>64</v>
+      </c>
+      <c r="G7" s="12">
+        <v>100</v>
+      </c>
+      <c r="H7" s="23"/>
+      <c r="I7" s="12">
+        <v>0.94889999999999997</v>
+      </c>
+      <c r="J7" s="12">
+        <v>1</v>
+      </c>
+      <c r="K7" s="12">
+        <v>0.58330000000000004</v>
+      </c>
+      <c r="L7" s="12">
+        <v>0.79090000000000005</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="O7" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="P7" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q7" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="R7" s="19"/>
+    </row>
+    <row r="8" spans="5:18" x14ac:dyDescent="0.35">
+      <c r="E8" s="8">
+        <v>28</v>
+      </c>
+      <c r="F8" s="8">
+        <v>64</v>
+      </c>
+      <c r="G8" s="8">
+        <v>100</v>
+      </c>
+      <c r="H8" s="23"/>
+      <c r="I8" s="17">
+        <v>0.98819999999999997</v>
+      </c>
+      <c r="J8" s="17">
+        <v>1</v>
+      </c>
+      <c r="K8" s="17">
+        <v>0.6431</v>
+      </c>
+      <c r="L8" s="17">
+        <v>0.7419</v>
+      </c>
+      <c r="M8" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="N8" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="O8" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="P8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q8" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="5:18" x14ac:dyDescent="0.35">
+      <c r="E9" s="8">
+        <v>29</v>
+      </c>
+      <c r="F9" s="8">
+        <v>64</v>
+      </c>
+      <c r="G9" s="8">
+        <v>100</v>
+      </c>
+      <c r="H9" s="23"/>
+      <c r="I9" s="17">
+        <v>0.98340000000000005</v>
+      </c>
+      <c r="J9" s="17">
+        <v>1</v>
+      </c>
+      <c r="K9" s="18">
+        <v>0.71950000000000003</v>
+      </c>
+      <c r="L9" s="17">
+        <v>0.75860000000000005</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="N9" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="O9" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="P9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q9" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="5:18" x14ac:dyDescent="0.35">
+      <c r="E10" s="8">
+        <v>30</v>
+      </c>
+      <c r="F10" s="8">
+        <v>64</v>
+      </c>
+      <c r="G10" s="8">
+        <v>100</v>
+      </c>
+      <c r="H10" s="23"/>
+      <c r="I10" s="17">
+        <v>0.40550000000000003</v>
+      </c>
+      <c r="J10" s="17">
+        <v>0.89119999999999999</v>
+      </c>
+      <c r="K10" s="17">
+        <v>0.33119999999999999</v>
+      </c>
+      <c r="L10" s="17">
+        <v>0.50790000000000002</v>
+      </c>
+      <c r="M10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="O10" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="P10" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q10" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="5:18" x14ac:dyDescent="0.35">
+      <c r="E11" s="8">
+        <v>31</v>
+      </c>
+      <c r="F11" s="8">
+        <v>64</v>
+      </c>
+      <c r="G11" s="8">
+        <v>100</v>
+      </c>
+      <c r="H11" s="23"/>
+      <c r="I11" s="17">
+        <v>0.99270000000000003</v>
+      </c>
+      <c r="J11" s="17">
+        <v>1</v>
+      </c>
+      <c r="K11" s="17">
+        <v>0.72370000000000001</v>
+      </c>
+      <c r="L11" s="17">
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="M11" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="N11" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="O11" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="P11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q11" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="5:18" x14ac:dyDescent="0.35">
+      <c r="E12" s="8">
+        <v>32</v>
+      </c>
+      <c r="F12" s="8">
+        <v>64</v>
+      </c>
+      <c r="G12" s="8">
+        <v>100</v>
+      </c>
+      <c r="H12" s="23"/>
+      <c r="I12" s="17">
+        <v>0.99629999999999996</v>
+      </c>
+      <c r="J12" s="17">
+        <v>1</v>
+      </c>
+      <c r="K12" s="17">
+        <v>0.74929999999999997</v>
+      </c>
+      <c r="L12" s="17">
+        <v>0.7752</v>
+      </c>
+      <c r="M12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="N12" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="O12" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="P12" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q12" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="5:18" x14ac:dyDescent="0.35">
+      <c r="E14" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="13">
+        <v>0.95579999999999998</v>
+      </c>
+      <c r="J14" s="13">
+        <v>1</v>
+      </c>
+      <c r="K14" s="13">
+        <v>0.69169999999999998</v>
+      </c>
+      <c r="L14" s="13">
+        <v>0.85750000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="O2:O4"/>
+    <mergeCell ref="P2:P4"/>
+    <mergeCell ref="Q2:Q4"/>
+    <mergeCell ref="R2:R4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="N2:N4"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="H5:H12"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>